<commit_message>
15 Nov 2021 commit
</commit_message>
<xml_diff>
--- a/src/main/java/ccpa/testdata/TestDataCCPA2.xlsx
+++ b/src/main/java/ccpa/testdata/TestDataCCPA2.xlsx
@@ -994,7 +994,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1333,8 +1333,8 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,7 +1453,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1537,7 +1537,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D14" t="s">
         <v>118</v>
@@ -1943,7 +1943,7 @@
         <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
23 Nov 2021 commit
</commit_message>
<xml_diff>
--- a/src/main/java/ccpa/testdata/TestDataCCPA2.xlsx
+++ b/src/main/java/ccpa/testdata/TestDataCCPA2.xlsx
@@ -994,7 +994,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1333,8 +1333,8 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,7 +2573,7 @@
         <v>108</v>
       </c>
       <c r="C88" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
         <v>192</v>

</xml_diff>